<commit_message>
atualizacao da modelagem de cadastro
</commit_message>
<xml_diff>
--- a/Documentacao/Modelagem de Cadastro.xlsx
+++ b/Documentacao/Modelagem de Cadastro.xlsx
@@ -1,18 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24004"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_4ACC360EE3F7EA409546A39069DA650C0924B790" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marlene\Desktop\CashFix\Documentacao\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63416ECC-5528-445A-B71F-53B716B7F0B1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="9495" windowHeight="3615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
     <sheet name="Plan2" sheetId="2" r:id="rId2"/>
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -238,9 +243,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -303,7 +308,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -335,47 +340,173 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -395,7 +526,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -718,219 +849,219 @@
   <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="64" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="3"/>
+    <col min="1" max="1" width="64" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="16"/>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="5" t="s">
+      <c r="B4" s="13"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="6">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="16">
         <v>0</v>
       </c>
-      <c r="B9" s="16"/>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="2"/>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="4" t="s">
+      <c r="B9" s="13"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="6"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="14"/>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="5" t="s">
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="14"/>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="6">
+      <c r="B12" s="18"/>
+      <c r="C12" s="3"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="16">
         <v>0</v>
       </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="14"/>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="5" t="s">
+      <c r="B13" s="13"/>
+      <c r="C13" s="3"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="5" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="16"/>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="5" t="s">
+      <c r="B16" s="18"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="16"/>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="5" t="s">
+      <c r="B17" s="18"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="16"/>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="5" t="s">
+      <c r="B18" s="18"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="16"/>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="5" t="s">
+      <c r="B19" s="13"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="5" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="15"/>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="5" t="s">
+      <c r="B22" s="20"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="15"/>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="5" t="s">
+      <c r="B23" s="20"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="15"/>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="5" t="s">
+      <c r="B24" s="20"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="15"/>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="9" t="s">
+      <c r="B25" s="21"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="9" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="15"/>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="9" t="s">
+      <c r="B28" s="20"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="8"/>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="10" t="s">
+      <c r="B29" s="25"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="5" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="19" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="5" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B34" s="15"/>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="5" t="s">
+      <c r="B34" s="20"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="15"/>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="5" t="s">
+      <c r="B35" s="20"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B36" s="15"/>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="5" t="s">
+      <c r="B36" s="20"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B37" s="8"/>
-    </row>
-    <row r="39" spans="1:2" ht="30">
-      <c r="A39" s="13" t="s">
+      <c r="B37" s="25"/>
+    </row>
+    <row r="39" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="12"/>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -954,7 +1085,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -966,25 +1097,25 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1102,13 +1233,34 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C32F43F-FB64-4638-A987-91A602FF22D7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{869BE4C8-1A76-4E79-B4DA-8EF14BDA902B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{869BE4C8-1A76-4E79-B4DA-8EF14BDA902B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C32F43F-FB64-4638-A987-91A602FF22D7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53153897-46F1-4546-8E63-443BD6CC87FA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53153897-46F1-4546-8E63-443BD6CC87FA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>